<commit_message>
refactor: Ajustar modelos y Excel según requerimientos
- Flores: Removida bodega (se compran según necesidad)
- Productos: Agregados campos detallados (colores, flores asociadas, 360/180, tamaño, cuidados)
- Pedidos: Agregados campos completos (nro Shopify, precio envío, destinatario, mensaje, firma, motivo)
- Excel regenerados con nuevas estructuras
- Agregada lista de motivos estándar
</commit_message>
<xml_diff>
--- a/01_Inventario_Flores.xlsx
+++ b/01_Inventario_Flores.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,10 +440,9 @@
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="10" customWidth="1" min="8" max="8"/>
-    <col width="18" customWidth="1" min="9" max="9"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -474,20 +473,15 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Cantidad Stock</t>
+          <t>Cantidad Stock Actual</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Bodega</t>
+          <t>Unidad</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Unidad</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Última Actualización</t>
         </is>
@@ -522,15 +516,10 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Bodega 1</t>
+          <t>Tallo</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
         <is>
           <t>2025-10-20</t>
         </is>
@@ -565,15 +554,10 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Bodega 1</t>
+          <t>Tallo</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
         <is>
           <t>2025-10-20</t>
         </is>
@@ -608,15 +592,10 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Bodega 1</t>
+          <t>Tallo</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
         <is>
           <t>2025-10-20</t>
         </is>
@@ -651,15 +630,10 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Bodega 2</t>
+          <t>Tallo</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
         <is>
           <t>2025-10-21</t>
         </is>
@@ -694,15 +668,10 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Bodega 1</t>
+          <t>Tallo</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
         <is>
           <t>2025-10-19</t>
         </is>
@@ -737,15 +706,10 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Bodega 1</t>
+          <t>Tallo</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
         <is>
           <t>2025-10-19</t>
         </is>
@@ -780,15 +744,10 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Bodega 2</t>
+          <t>Tallo</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
         <is>
           <t>2025-10-22</t>
         </is>
@@ -823,15 +782,10 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Bodega 1</t>
+          <t>Tallo</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
         <is>
           <t>2025-10-20</t>
         </is>
@@ -866,15 +820,10 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Bodega 1</t>
+          <t>Tallo</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
         <is>
           <t>2025-10-20</t>
         </is>
@@ -909,15 +858,10 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Bodega 2</t>
+          <t>Tallo</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
         <is>
           <t>2025-10-20</t>
         </is>
@@ -952,15 +896,10 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Bodega 1</t>
+          <t>Tallo</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
         <is>
           <t>2025-10-18</t>
         </is>
@@ -995,15 +934,10 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Bodega 1</t>
+          <t>Tallo</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
         <is>
           <t>2025-10-18</t>
         </is>
@@ -1038,15 +972,10 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Bodega 2</t>
+          <t>Ramo</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
-        <is>
-          <t>Ramo</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
         <is>
           <t>2025-10-21</t>
         </is>
@@ -1081,15 +1010,10 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Bodega 2</t>
+          <t>Ramo</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
-        <is>
-          <t>Ramo</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
         <is>
           <t>2025-10-21</t>
         </is>
@@ -1124,15 +1048,10 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Bodega 1</t>
+          <t>Tallo</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
         <is>
           <t>2025-10-20</t>
         </is>
@@ -1167,15 +1086,10 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Bodega 1</t>
+          <t>Tallo</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
         <is>
           <t>2025-10-20</t>
         </is>
@@ -1210,15 +1124,10 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Bodega 2</t>
+          <t>Tallo</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
         <is>
           <t>2025-10-19</t>
         </is>
@@ -1253,15 +1162,10 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Bodega 1</t>
+          <t>Tallo</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
         <is>
           <t>2025-10-22</t>
         </is>
@@ -1296,15 +1200,10 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Bodega 1</t>
+          <t>Rama</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
-        <is>
-          <t>Rama</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
         <is>
           <t>2025-10-21</t>
         </is>
@@ -1339,15 +1238,10 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Bodega 2</t>
+          <t>Rama</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
-        <is>
-          <t>Rama</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
         <is>
           <t>2025-10-20</t>
         </is>

</xml_diff>

<commit_message>
feat: Sistema completo de gestión de fotos
- Agregada columna 'Foto' a todos los Excel (flores, contenedores, productos)
- Modelos actualizados con campo foto_url
- API completa para subir/actualizar/eliminar fotos
- Componente React ImageUpload reutilizable
- Tarjetas del tablero muestran foto del producto
- Soporte para JPG, PNG, GIF, WebP
- Validación de tamaño (max 5MB)
- Carpeta backend/uploads para almacenar imágenes
</commit_message>
<xml_diff>
--- a/01_Inventario_Flores.xlsx
+++ b/01_Inventario_Flores.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,11 +438,12 @@
     <col width="8" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
-    <col width="10" customWidth="1" min="7" max="7"/>
-    <col width="18" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="18" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -463,25 +464,30 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Foto</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Proveedor</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Costo Unitario</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Cantidad Stock Actual</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Unidad</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Última Actualización</t>
         </is>
@@ -505,21 +511,26 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>rosa-roja.jpg</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>Flores del Valle</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>1500</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>120</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>Tallo</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>2025-10-20</t>
         </is>
@@ -543,21 +554,26 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>rosa-blanca.jpg</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>Flores del Valle</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>1500</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>85</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
       <c r="H3" t="inlineStr">
+        <is>
+          <t>Tallo</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>2025-10-20</t>
         </is>
@@ -581,21 +597,26 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>rosa-rosada.jpg</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>Flores del Valle</t>
         </is>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>1500</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>95</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
       <c r="H4" t="inlineStr">
+        <is>
+          <t>Tallo</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>2025-10-20</t>
         </is>
@@ -619,21 +640,26 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>rosa-amarilla.jpg</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Flores del Valle</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>1500</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>60</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
       <c r="H5" t="inlineStr">
+        <is>
+          <t>Tallo</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>2025-10-21</t>
         </is>
@@ -657,21 +683,26 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>lirio-blanco.jpg</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>Jardín Central</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>2500</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>45</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
       <c r="H6" t="inlineStr">
+        <is>
+          <t>Tallo</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>2025-10-19</t>
         </is>
@@ -695,21 +726,26 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>lirio-rosado.jpg</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>Jardín Central</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>2500</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>38</v>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
       <c r="H7" t="inlineStr">
+        <is>
+          <t>Tallo</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
         <is>
           <t>2025-10-19</t>
         </is>
@@ -733,21 +769,26 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>girasol.jpg</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>Campo Florido</t>
         </is>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>2000</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>30</v>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
       <c r="H8" t="inlineStr">
+        <is>
+          <t>Tallo</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
         <is>
           <t>2025-10-22</t>
         </is>
@@ -771,21 +812,26 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>clavel-rojo.jpg</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>Flores del Valle</t>
         </is>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>800</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>150</v>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
       <c r="H9" t="inlineStr">
+        <is>
+          <t>Tallo</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
         <is>
           <t>2025-10-20</t>
         </is>
@@ -809,21 +855,26 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
+          <t>clavel-blanco.jpg</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>Flores del Valle</t>
         </is>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>800</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>140</v>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
       <c r="H10" t="inlineStr">
+        <is>
+          <t>Tallo</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
         <is>
           <t>2025-10-20</t>
         </is>
@@ -847,21 +898,26 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>clavel-rosado.jpg</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>Flores del Valle</t>
         </is>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>800</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>130</v>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
       <c r="H11" t="inlineStr">
+        <is>
+          <t>Tallo</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
         <is>
           <t>2025-10-20</t>
         </is>
@@ -885,21 +941,26 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
+          <t>tulipan-rojo.jpg</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>Jardín Central</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>2200</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>25</v>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
       <c r="H12" t="inlineStr">
+        <is>
+          <t>Tallo</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
         <is>
           <t>2025-10-18</t>
         </is>
@@ -923,21 +984,26 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
+          <t>tulipan-amarillo.jpg</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>Jardín Central</t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>2200</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>20</v>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
       <c r="H13" t="inlineStr">
+        <is>
+          <t>Tallo</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>2025-10-18</t>
         </is>
@@ -961,21 +1027,26 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
+          <t>hortensia-azul.jpg</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>Campo Florido</t>
         </is>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>3500</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>15</v>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>Ramo</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>2025-10-21</t>
         </is>
@@ -999,21 +1070,26 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
+          <t>hortensia-rosada.jpg</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>Campo Florido</t>
         </is>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>3500</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>18</v>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>Ramo</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>2025-10-21</t>
         </is>
@@ -1037,21 +1113,26 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
+          <t>gerbera-naranja.jpg</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>Flores del Valle</t>
         </is>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>1800</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>55</v>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
       <c r="H16" t="inlineStr">
+        <is>
+          <t>Tallo</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
         <is>
           <t>2025-10-20</t>
         </is>
@@ -1075,21 +1156,26 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
+          <t>gerbera-rosada.jpg</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>Flores del Valle</t>
         </is>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>1800</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>48</v>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
       <c r="H17" t="inlineStr">
+        <is>
+          <t>Tallo</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
         <is>
           <t>2025-10-20</t>
         </is>
@@ -1113,21 +1199,26 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>orquidea-blanca.jpg</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>Jardín Central</t>
         </is>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>5000</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>12</v>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
       <c r="H18" t="inlineStr">
+        <is>
+          <t>Tallo</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
         <is>
           <t>2025-10-19</t>
         </is>
@@ -1151,21 +1242,26 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
+          <t>alstroemeria-morada.jpg</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>Campo Florido</t>
         </is>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>1200</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>70</v>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Tallo</t>
-        </is>
-      </c>
       <c r="H19" t="inlineStr">
+        <is>
+          <t>Tallo</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
         <is>
           <t>2025-10-22</t>
         </is>
@@ -1189,21 +1285,26 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
+          <t>eucalipto.jpg</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
           <t>Campo Florido</t>
         </is>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>500</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>200</v>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>Rama</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>2025-10-21</t>
         </is>
@@ -1227,21 +1328,26 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
+          <t>solidago.jpg</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
           <t>Flores del Valle</t>
         </is>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>600</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>100</v>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>Rama</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>2025-10-20</t>
         </is>

</xml_diff>